<commit_message>
ART-42 fixed the whitelist application and styling issues
</commit_message>
<xml_diff>
--- a/art/Example - Zugriffsmuster.xlsx
+++ b/art/Example - Zugriffsmuster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\merli\OneDrive\Dokumente\Softwareprojekt\art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF65AC0-BEEC-4765-B780-9DF445DB8DB6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BCF96D-F40C-4A5B-A0CC-EA49EE861C3B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="19245" xr2:uid="{B168051A-7169-2D49-AA3C-A7B0D258D96C}"/>
   </bookViews>
@@ -904,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA95D98-5EC8-C84E-BC9F-776C44071DBD}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I40" sqref="A13:I40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>